<commit_message>
Test results and drawio plots added.
</commit_message>
<xml_diff>
--- a/result/20220421133455_hist72_pred1_modelDNN1_epoch30_trainBusan/실험결과표2.xlsx
+++ b/result/20220421133455_hist72_pred1_modelDNN1_epoch30_trainBusan/실험결과표2.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="26" documentId="8_{89E126D1-9A66-4A6A-9F32-C68D80120653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89AA27BE-87A9-452F-BAC9-DD89B94A1CFA}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="-8580" windowWidth="16200" windowHeight="14175" xr2:uid="{2766BBED-68F4-4731-84E2-EF293B81F3CB}"/>
+    <workbookView xWindow="-16200" yWindow="5595" windowWidth="16200" windowHeight="14175" xr2:uid="{2766BBED-68F4-4731-84E2-EF293B81F3CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12:S18"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>